<commit_message>
Added ElementHelper class for finding elements and added tests as suggested for Footer
</commit_message>
<xml_diff>
--- a/test-data/footer-data.xlsx
+++ b/test-data/footer-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cgov_workspace\cgov-digital-platform-qa\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24E7276-1B9A-4A3D-A00D-D368B8EAD637}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663923C3-4861-4330-88CA-93973B184F08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="6860" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>path</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Spanish</t>
+  </si>
+  <si>
+    <t>/news-events/press-releases/2018/oropharyngeal-hpv-cisplatin</t>
   </si>
 </sst>
 </file>
@@ -437,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.08203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -523,6 +526,17 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed Back to top tests,combined two data providers into one and added test for language of Footer
</commit_message>
<xml_diff>
--- a/test-data/footer-data.xlsx
+++ b/test-data/footer-data.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cgov_workspace\cgov-digital-platform-qa\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663923C3-4861-4330-88CA-93973B184F08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF7F70E-5A5A-45AA-8262-BB819EA5B8A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6860" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6860" windowHeight="8250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_footer" sheetId="1" r:id="rId1"/>
-    <sheet name="pages_with_footer_spanish" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>path</t>
   </si>
@@ -43,9 +42,6 @@
     <t>Press Release</t>
   </si>
   <si>
-    <t>Blog Post</t>
-  </si>
-  <si>
     <t>language</t>
   </si>
   <si>
@@ -61,34 +57,31 @@
     <t>Cancer Center</t>
   </si>
   <si>
-    <t>/node/31</t>
-  </si>
-  <si>
     <t>PDQ Cancer Information Summary</t>
   </si>
   <si>
     <t>types/breast/patient/breast-treatment-pdq</t>
   </si>
   <si>
-    <t>node/56</t>
-  </si>
-  <si>
-    <t>Home and Landing</t>
-  </si>
-  <si>
-    <t>Biography</t>
-  </si>
-  <si>
-    <t>node/26</t>
-  </si>
-  <si>
-    <t>espanol/node/56</t>
-  </si>
-  <si>
     <t>Spanish</t>
   </si>
   <si>
     <t>/news-events/press-releases/2018/oropharyngeal-hpv-cisplatin</t>
+  </si>
+  <si>
+    <t>espanol/cancer/sobrellevar/sentimientos/hoja-informativa-estres</t>
+  </si>
+  <si>
+    <t>about-cancer/coping/feelings/relaxation/hpv-vaccine-presidents-cancer-panel-improving-uptake</t>
+  </si>
+  <si>
+    <t>Blog</t>
+  </si>
+  <si>
+    <t>about-cancer/coping/feelings/relaxation/vitamin-d-supplement-cancer-prevention</t>
+  </si>
+  <si>
+    <t>Blog Page</t>
   </si>
 </sst>
 </file>
@@ -124,8 +117,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.08203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -460,62 +459,62 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -523,73 +522,43 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABFCDDC7-4B99-4B0D-9AF6-16B3D00936FD}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.08203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="37.58203125" customWidth="1"/>
-    <col min="2" max="2" width="29.58203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
+      <c r="C10" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>